<commit_message>
feat: Add Dijkstra Class And Modify Assignment 2
다익스트라 클래스 구현 및 과제 2번 수정
</commit_message>
<xml_diff>
--- a/0502_Assignment/문제 해결 과정.xlsx
+++ b/0502_Assignment/문제 해결 과정.xlsx
@@ -182,7 +182,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -267,13 +267,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -290,6 +283,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>562516</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="428625"/>
+          <a:ext cx="3877216" cy="4429743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -557,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1839,5 +1875,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>